<commit_message>
Updated load_data.py to update existing or add new records
</commit_message>
<xml_diff>
--- a/data/sample1.xlsx
+++ b/data/sample1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/move_on/django/projects/myproject/myproject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4540765-5179-3441-8447-A05241125B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4344DF4-3E89-1E48-932C-F8F3B822E0C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15740" xr2:uid="{92571465-E93C-C148-8E05-745810DC96BC}"/>
+    <workbookView xWindow="780" yWindow="820" windowWidth="27640" windowHeight="15740" xr2:uid="{92571465-E93C-C148-8E05-745810DC96BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="200">
   <si>
     <t>Chapter Number</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Caption</t>
   </si>
   <si>
-    <t>Source1</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>F30</t>
-  </si>
-  <si>
-    <t>Infant incubator</t>
   </si>
   <si>
     <t>Dräger Medical</t>
@@ -625,6 +619,21 @@
   </si>
   <si>
     <t>CaseStudy</t>
+  </si>
+  <si>
+    <t>Infant incubator1</t>
+  </si>
+  <si>
+    <t>F21</t>
+  </si>
+  <si>
+    <t>2234567890123_CH13_FIGF21</t>
+  </si>
+  <si>
+    <t>Dräger Medicals</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -1172,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E6C815-22E3-9C40-A32F-55E935A55CFA}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,1529 +1200,1566 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="L2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="M2" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>28</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="L3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="398" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="D4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="F4" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>34</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="L4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="E5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="F8" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>51</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="342" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="D9" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="E9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="314" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>61</v>
-      </c>
       <c r="E10" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="314" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
         <v>66</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="314" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="370" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="E13" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="G13" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="H13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" t="s">
         <v>76</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="384" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="E14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="G14" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="18" t="s">
+      <c r="H14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" t="s">
         <v>82</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="E15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="D17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="328" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="E18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>103</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="238" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="E19" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="180" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>112</v>
-      </c>
       <c r="E20" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="180" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="D21" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>118</v>
-      </c>
       <c r="E21" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="12"/>
       <c r="H21" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="D22" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="H22" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22" s="25" t="s">
+      <c r="L22" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" t="s">
         <v>122</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="L22" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>127</v>
-      </c>
       <c r="D23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I23" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="L23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K23" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="H24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" t="s">
         <v>130</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M24" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="L25" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K25" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I26" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="L26" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I27" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="L27" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K27" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A28" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="E28" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="L28" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K28" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="L29" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K29" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D30" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I30" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="L30" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K30" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I31" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="L31" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K31" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D32" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L32" s="13"/>
       <c r="M32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="D33" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>161</v>
-      </c>
       <c r="E33" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="12"/>
       <c r="H33" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L33" s="13"/>
       <c r="M33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>160</v>
-      </c>
       <c r="D34" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L34" s="13"/>
       <c r="M34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L35" s="13"/>
       <c r="M35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" s="11" t="s">
+      <c r="E36" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L36" s="13"/>
       <c r="M36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>178</v>
-      </c>
       <c r="E37" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L37" s="13"/>
       <c r="M37" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="E38" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="G38" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="E38" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>185</v>
-      </c>
       <c r="H38" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L38" s="13"/>
       <c r="M38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>189</v>
-      </c>
       <c r="D39" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L39" s="13"/>
       <c r="M39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="255" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="E40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="G40" s="12"/>
       <c r="H40" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L40" s="13"/>
       <c r="M40" t="s">
-        <v>195</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="255" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G41" s="12"/>
+      <c r="H41" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41" s="13"/>
+      <c r="M41" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2788,6 +2834,7 @@
     <hyperlink ref="I39" r:id="rId68" xr:uid="{2AC25DC0-313C-744C-AE7B-71EEFAD4CB0E}"/>
     <hyperlink ref="I40" r:id="rId69" xr:uid="{3BDD8D6B-3F94-5E48-A56E-3FDC6BD07E5E}"/>
     <hyperlink ref="I3" r:id="rId70" xr:uid="{B37FA0EC-5A93-1841-AF36-A36B2A1176D5}"/>
+    <hyperlink ref="I41" r:id="rId71" xr:uid="{A3531AB7-AE5E-8045-A59E-7EA25F037F14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>